<commit_message>
añadido excel sus y excel review
</commit_message>
<xml_diff>
--- a/P4/Cuestionario SUS DIU Incompleto.xlsx
+++ b/P4/Cuestionario SUS DIU Incompleto.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romer\OneDrive\Desktop\UGR\tercero\Segundo cuatrimestre\DIU\Practica4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E33C04A-C762-416A-AEFB-6B63AC4F2471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1DD5AC-E011-4FAF-8E68-DBC1B63FDFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
   <si>
     <t xml:space="preserve">DISEÑO DE INTERFACES DE USUARIO </t>
   </si>
@@ -284,9 +284,6 @@
     <t>EQUIPO:  Dumbledore               24/05/2023</t>
   </si>
   <si>
-    <t>TEST B: La alborea</t>
-  </si>
-  <si>
     <t>Mujer</t>
   </si>
   <si>
@@ -414,6 +411,15 @@
   </si>
   <si>
     <t>Está estudiando en Granada y decide buscar una actividad nueva para hacer con sus amigos, está cansado ya que ha dormido poco por los exámenes</t>
+  </si>
+  <si>
+    <t>Quiere buscar nuevas actividades para sus eventos y quiere probar con el flamenco en Granada. Está indiferente ya que no conoce el flamenco y no espera nada en concreto.</t>
+  </si>
+  <si>
+    <t>Al ser azafata tiene dos días libres en Granada y organiza con sus compañeros una visita para conocer la historia de Granada. Debido a su pasión por la historia está intrigada por la ruta.</t>
+  </si>
+  <si>
+    <t>TEST B</t>
   </si>
 </sst>
 </file>
@@ -1181,10 +1187,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O1007"/>
+  <dimension ref="A1:P1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1194,32 +1200,33 @@
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" hidden="1" customWidth="1"/>
     <col min="5" max="15" width="27.85546875" customWidth="1"/>
+    <col min="16" max="16" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -1242,7 +1249,7 @@
       <c r="N3" s="49"/>
       <c r="O3" s="6"/>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
@@ -1260,10 +1267,10 @@
         <v>8</v>
       </c>
       <c r="H4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>59</v>
       </c>
       <c r="J4" s="50" t="s">
         <v>5</v>
@@ -1278,51 +1285,51 @@
         <v>8</v>
       </c>
       <c r="N4" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="O4" s="39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="38"/>
       <c r="J5" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K5" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L5" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M5" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N5" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O5" s="39"/>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1360,121 +1367,121 @@
       </c>
       <c r="O6" s="11"/>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="38"/>
       <c r="J7" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K7" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L7" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M7" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N7" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O7" s="39"/>
     </row>
-    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I8" s="38"/>
       <c r="J8" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L8" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N8" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O8" s="39"/>
     </row>
-    <row r="9" spans="1:15" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="43" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="H9" s="52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" s="43"/>
       <c r="J9" s="40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K9" s="43" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="L9" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M9" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N9" s="52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O9" s="42"/>
     </row>
-    <row r="10" spans="1:15" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
       <c r="E10" s="14"/>
@@ -1486,7 +1493,7 @@
       <c r="K10" s="14"/>
       <c r="O10" s="16"/>
     </row>
-    <row r="11" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="13" t="s">
         <v>14</v>
       </c>
@@ -1524,7 +1531,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="13" t="s">
         <v>15</v>
       </c>
@@ -1563,7 +1570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="18" t="s">
         <v>16</v>
@@ -1581,13 +1588,13 @@
         <v>20</v>
       </c>
       <c r="G13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="I13" s="21" t="s">
         <v>61</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>62</v>
       </c>
       <c r="J13" s="22" t="s">
         <v>17</v>
@@ -1599,16 +1606,19 @@
         <v>20</v>
       </c>
       <c r="M13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="O13" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="O13" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P13" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23">
         <v>1</v>
       </c>
@@ -1616,33 +1626,46 @@
         <v>21</v>
       </c>
       <c r="C14" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14" s="26">
         <f>C14-1</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="44">
+        <v>3</v>
+      </c>
+      <c r="E14" s="27">
         <v>4</v>
       </c>
-      <c r="G14" s="44"/>
+      <c r="F14" s="47">
+        <v>5</v>
+      </c>
+      <c r="G14" s="44">
+        <v>5</v>
+      </c>
       <c r="H14" s="44">
+        <v>5</v>
+      </c>
+      <c r="I14" s="44"/>
+      <c r="J14" s="28">
         <v>4</v>
       </c>
-      <c r="I14" s="44"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="47">
-        <v>5</v>
-      </c>
-      <c r="M14" s="44"/>
-      <c r="N14" s="47">
-        <v>5</v>
+      <c r="K14" s="27">
+        <v>3</v>
+      </c>
+      <c r="L14" s="44">
+        <v>4</v>
+      </c>
+      <c r="M14" s="44">
+        <v>4</v>
+      </c>
+      <c r="N14" s="44">
+        <v>4</v>
       </c>
       <c r="O14" s="48"/>
-    </row>
-    <row r="15" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P14" s="24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23">
         <v>2</v>
       </c>
@@ -1656,27 +1679,40 @@
         <f>5-C15</f>
         <v>4</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="44">
+      <c r="E15" s="27">
         <v>2</v>
       </c>
-      <c r="G15" s="44"/>
+      <c r="F15" s="47">
+        <v>2</v>
+      </c>
+      <c r="G15" s="44">
+        <v>2</v>
+      </c>
       <c r="H15" s="44">
+        <v>2</v>
+      </c>
+      <c r="I15" s="44"/>
+      <c r="J15" s="28">
+        <v>2</v>
+      </c>
+      <c r="K15" s="27">
         <v>1</v>
       </c>
-      <c r="I15" s="44"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="47">
+      <c r="L15" s="44">
         <v>2</v>
       </c>
-      <c r="M15" s="44"/>
-      <c r="N15" s="47">
+      <c r="M15" s="44">
         <v>2</v>
       </c>
+      <c r="N15" s="44">
+        <v>1</v>
+      </c>
       <c r="O15" s="48"/>
-    </row>
-    <row r="16" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P15" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="23">
         <v>3</v>
       </c>
@@ -1690,27 +1726,40 @@
         <f>C16-1</f>
         <v>3</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="44">
+      <c r="E16" s="27">
+        <v>3</v>
+      </c>
+      <c r="F16" s="47">
         <v>4</v>
       </c>
-      <c r="G16" s="44"/>
+      <c r="G16" s="44">
+        <v>3</v>
+      </c>
       <c r="H16" s="44">
         <v>5</v>
       </c>
       <c r="I16" s="44"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="47">
+      <c r="J16" s="28">
         <v>4</v>
       </c>
-      <c r="M16" s="44"/>
-      <c r="N16" s="47">
+      <c r="K16" s="27">
+        <v>4</v>
+      </c>
+      <c r="L16" s="44">
+        <v>4</v>
+      </c>
+      <c r="M16" s="44">
         <v>5</v>
       </c>
+      <c r="N16" s="44">
+        <v>5</v>
+      </c>
       <c r="O16" s="48"/>
-    </row>
-    <row r="17" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P16" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="23">
         <v>4</v>
       </c>
@@ -1724,27 +1773,40 @@
         <f>5-C17</f>
         <v>3</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="44">
+      <c r="E17" s="27">
         <v>1</v>
       </c>
-      <c r="G17" s="44"/>
+      <c r="F17" s="47">
+        <v>2</v>
+      </c>
+      <c r="G17" s="44">
+        <v>1</v>
+      </c>
       <c r="H17" s="44">
         <v>1</v>
       </c>
       <c r="I17" s="44"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="47">
-        <v>2</v>
-      </c>
-      <c r="M17" s="44"/>
-      <c r="N17" s="47">
+      <c r="J17" s="28">
+        <v>3</v>
+      </c>
+      <c r="K17" s="27">
         <v>1</v>
       </c>
+      <c r="L17" s="44">
+        <v>1</v>
+      </c>
+      <c r="M17" s="44">
+        <v>1</v>
+      </c>
+      <c r="N17" s="44">
+        <v>1</v>
+      </c>
       <c r="O17" s="48"/>
-    </row>
-    <row r="18" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P17" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23">
         <v>5</v>
       </c>
@@ -1758,27 +1820,40 @@
         <f>C18-1</f>
         <v>4</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="44">
+      <c r="E18" s="27">
         <v>5</v>
       </c>
-      <c r="G18" s="44"/>
+      <c r="F18" s="47">
+        <v>5</v>
+      </c>
+      <c r="G18" s="44">
+        <v>5</v>
+      </c>
       <c r="H18" s="44">
         <v>5</v>
       </c>
       <c r="I18" s="44"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="47">
+      <c r="J18" s="28">
         <v>5</v>
       </c>
-      <c r="M18" s="44"/>
-      <c r="N18" s="47">
+      <c r="K18" s="27">
         <v>5</v>
       </c>
+      <c r="L18" s="44">
+        <v>5</v>
+      </c>
+      <c r="M18" s="44">
+        <v>5</v>
+      </c>
+      <c r="N18" s="44">
+        <v>5</v>
+      </c>
       <c r="O18" s="48"/>
-    </row>
-    <row r="19" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P18" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="23">
         <v>6</v>
       </c>
@@ -1792,27 +1867,40 @@
         <f>5-C19</f>
         <v>3</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="44">
+      <c r="E19" s="27">
         <v>1</v>
       </c>
-      <c r="G19" s="44"/>
+      <c r="F19" s="47">
+        <v>1</v>
+      </c>
+      <c r="G19" s="44">
+        <v>1</v>
+      </c>
       <c r="H19" s="44">
         <v>1</v>
       </c>
       <c r="I19" s="44"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="47">
+      <c r="J19" s="28">
+        <v>2</v>
+      </c>
+      <c r="K19" s="27">
         <v>1</v>
       </c>
-      <c r="M19" s="44"/>
-      <c r="N19" s="47">
+      <c r="L19" s="44">
         <v>1</v>
       </c>
+      <c r="M19" s="44">
+        <v>1</v>
+      </c>
+      <c r="N19" s="44">
+        <v>1</v>
+      </c>
       <c r="O19" s="48"/>
-    </row>
-    <row r="20" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P19" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23">
         <v>7</v>
       </c>
@@ -1826,27 +1914,40 @@
         <f>C20-1</f>
         <v>3</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="44">
+      <c r="E20" s="27">
+        <v>3</v>
+      </c>
+      <c r="F20" s="47">
         <v>5</v>
       </c>
-      <c r="G20" s="44"/>
+      <c r="G20" s="44">
+        <v>2</v>
+      </c>
       <c r="H20" s="44">
         <v>5</v>
       </c>
       <c r="I20" s="44"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="47">
+      <c r="J20" s="28">
+        <v>4</v>
+      </c>
+      <c r="K20" s="27">
+        <v>4</v>
+      </c>
+      <c r="L20" s="44">
         <v>5</v>
       </c>
-      <c r="M20" s="44"/>
-      <c r="N20" s="47">
+      <c r="M20" s="44">
+        <v>4</v>
+      </c>
+      <c r="N20" s="44">
         <v>5</v>
       </c>
       <c r="O20" s="48"/>
-    </row>
-    <row r="21" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P20" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="23">
         <v>8</v>
       </c>
@@ -1860,27 +1961,40 @@
         <f>5-C21</f>
         <v>2</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="44">
+      <c r="E21" s="27">
+        <v>3</v>
+      </c>
+      <c r="F21" s="47">
+        <v>4</v>
+      </c>
+      <c r="G21" s="44">
+        <v>3</v>
+      </c>
+      <c r="H21" s="44">
+        <v>3</v>
+      </c>
+      <c r="I21" s="44"/>
+      <c r="J21" s="28">
+        <v>3</v>
+      </c>
+      <c r="K21" s="27">
+        <v>3</v>
+      </c>
+      <c r="L21" s="44">
         <v>2</v>
       </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44">
+      <c r="M21" s="44">
+        <v>2</v>
+      </c>
+      <c r="N21" s="44">
         <v>1</v>
       </c>
-      <c r="I21" s="44"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="47">
-        <v>4</v>
-      </c>
-      <c r="M21" s="44"/>
-      <c r="N21" s="47">
-        <v>1</v>
-      </c>
       <c r="O21" s="48"/>
-    </row>
-    <row r="22" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P21" s="24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23">
         <v>9</v>
       </c>
@@ -1894,27 +2008,40 @@
         <f>C22-1</f>
         <v>1</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="44">
+      <c r="E22" s="27">
+        <v>3</v>
+      </c>
+      <c r="F22" s="47">
         <v>4</v>
       </c>
-      <c r="G22" s="44"/>
+      <c r="G22" s="44">
+        <v>3</v>
+      </c>
       <c r="H22" s="44">
         <v>5</v>
       </c>
       <c r="I22" s="44"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="47">
+      <c r="J22" s="28">
+        <v>3</v>
+      </c>
+      <c r="K22" s="27">
         <v>4</v>
       </c>
-      <c r="M22" s="44"/>
-      <c r="N22" s="47">
+      <c r="L22" s="44">
+        <v>4</v>
+      </c>
+      <c r="M22" s="44">
+        <v>4</v>
+      </c>
+      <c r="N22" s="44">
         <v>5</v>
       </c>
       <c r="O22" s="48"/>
-    </row>
-    <row r="23" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P22" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="23">
         <v>10</v>
       </c>
@@ -1928,54 +2055,67 @@
         <f>5-C23</f>
         <v>3</v>
       </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="44">
+      <c r="E23" s="27">
+        <v>2</v>
+      </c>
+      <c r="F23" s="47">
         <v>1</v>
       </c>
-      <c r="G23" s="44"/>
+      <c r="G23" s="44">
+        <v>2</v>
+      </c>
       <c r="H23" s="44">
         <v>1</v>
       </c>
       <c r="I23" s="44"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="47">
+      <c r="J23" s="28">
+        <v>3</v>
+      </c>
+      <c r="K23" s="27">
+        <v>2</v>
+      </c>
+      <c r="L23" s="44">
         <v>1</v>
       </c>
-      <c r="M23" s="44"/>
-      <c r="N23" s="47">
+      <c r="M23" s="44">
         <v>1</v>
       </c>
+      <c r="N23" s="44">
+        <v>1</v>
+      </c>
       <c r="O23" s="48"/>
-    </row>
-    <row r="24" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P23" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
       <c r="B24" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="29">
         <f>((C14-1)+(5-C15)+(C16-1)+(5-C17)+(C18-1)+(5-C19)+(C20-1)+(5-C21)+(C22-1)+(5-C23))*2.5</f>
-        <v>67.5</v>
+        <v>72.5</v>
       </c>
       <c r="D24" s="30">
         <f>(SUM(D14:D23))*2.5</f>
-        <v>67.5</v>
+        <v>72.5</v>
       </c>
       <c r="E24" s="31">
         <f t="shared" ref="E24:M24" si="0">((E14-1)+(5-E15)+(E16-1)+(5-E17)+(E18-1)+(5-E19)+(E20-1)+(5-E21)+(E22-1)+(5-E23))*2.5</f>
-        <v>50</v>
+        <v>72.5</v>
       </c>
       <c r="F24" s="31">
         <f t="shared" si="0"/>
-        <v>87.5</v>
+        <v>82.5</v>
       </c>
       <c r="G24" s="31">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>72.5</v>
       </c>
       <c r="H24" s="31">
-        <f t="shared" si="0"/>
-        <v>97.5</v>
+        <f>((H14-1)+(5-H15)+(H16-1)+(5-H17)+(H18-1)+(5-H19)+(H20-1)+(5-H21)+(H22-1)+(5-H23))*2.5</f>
+        <v>92.5</v>
       </c>
       <c r="I24" s="31">
         <f t="shared" si="0"/>
@@ -1983,19 +2123,19 @@
       </c>
       <c r="J24" s="32">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>67.5</v>
       </c>
       <c r="K24" s="46">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="L24" s="46">
         <f t="shared" si="0"/>
-        <v>82.5</v>
+        <v>87.5</v>
       </c>
       <c r="M24" s="46">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>87.5</v>
       </c>
       <c r="N24" s="46">
         <f>((N14-1)+(5-N15)+(N16-1)+(5-N17)+(N18-1)+(5-N19)+(N20-1)+(5-N21)+(N22-1)+(5-N23))*2.5</f>
@@ -2005,65 +2145,91 @@
         <f>((O14-1)+(5-O15)+(O16-1)+(5-O17)+(O18-1)+(5-O19)+(O20-1)+(5-O21)+(O22-1)+(5-O23))*2.5</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="P24" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B25" s="34" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="34" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26" s="47"/>
+      <c r="L26" s="44"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27" s="47"/>
+      <c r="L27" s="44"/>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="47"/>
+      <c r="L28" s="44"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29" s="47"/>
+      <c r="L29" s="44"/>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="47"/>
+      <c r="L30" s="44"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31" s="47"/>
+      <c r="L31" s="44"/>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H32" s="47"/>
+      <c r="L32" s="44"/>
+    </row>
+    <row r="33" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H33" s="47"/>
+      <c r="L33" s="44"/>
+    </row>
+    <row r="34" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="35" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="H34" s="47"/>
+      <c r="L34" s="44"/>
+    </row>
+    <row r="35" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H35" s="47"/>
+      <c r="L35" s="44"/>
+    </row>
+    <row r="36" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3031,7 +3197,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 1 and 5" sqref="C14:C23 E14:O23 J10" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 1 and 5" sqref="C14:C23 H26:H35 J10 L26:L35 E14:O23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>

</xml_diff>